<commit_message>
Add progress and other fixes
Set maximum carryover grade to C
Remove unoffered carryovers
Modify summary generation
Move tasks to background execution
</commit_message>
<xml_diff>
--- a/static/excel/samples/Bio data sample.xlsx
+++ b/static/excel/samples/Bio data sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC6D22F-1E51-4E6D-BF7C-918A9633A24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C24E1C5-DA98-4FFD-81F3-9BA7128C56A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>Matric NO</t>
   </si>
@@ -67,9 +67,6 @@
     <t>MEG</t>
   </si>
   <si>
-    <t>Department Code</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -200,6 +197,12 @@
   </si>
   <si>
     <t>ORDU</t>
+  </si>
+  <si>
+    <t>Ogochukwu</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
 </sst>
 </file>
@@ -525,9 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -555,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -581,243 +582,246 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>36</v>
-      </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
-      </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>53</v>
-      </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>